<commit_message>
:truck: data from Paul
</commit_message>
<xml_diff>
--- a/demo/Antibiotics_2006.xlsx
+++ b/demo/Antibiotics_2006.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteo/Coding/Epistasis_Calculator/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B529043-2AFF-654E-904A-899AD4969404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C8FD9E-430F-F84A-8CB7-089B26314100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="1780" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="35">
   <si>
     <t>A42G</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>2900.0</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -487,12 +490,15 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>